<commit_message>
compare 5 datasets of death
</commit_message>
<xml_diff>
--- a/Data/cc-d-01.04.02.01.03.xlsx
+++ b/Data/cc-d-01.04.02.01.03.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\adb.intra.admin.ch\BFS$\Archive\BB\DEM\101_BEVNAT\Monatsauswertung\2020 - Monatsauswertung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\BB\DEM\101_BEVNAT\Monatsauswertung\2020 - Monatsauswertung\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6756"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6756" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Januar 2020p" sheetId="1" r:id="rId1"/>
+    <sheet name="Februar 2020p" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Februar 2020p'!$A$1:$H$61</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Januar 2020p'!$A$1:$H$61</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="62">
   <si>
     <t>cc-d-01.04.02.01.03</t>
   </si>
@@ -207,6 +209,12 @@
   </si>
   <si>
     <t>Stand am 10.03.2020</t>
+  </si>
+  <si>
+    <t>Todesfälle nach Kanton, Februar 2020</t>
+  </si>
+  <si>
+    <t>Stand am 09.04.2020</t>
   </si>
 </sst>
 </file>
@@ -551,8 +559,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Modele-BFSAktuell-Bevnat-Annuel-19.05.2009" xfId="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -568,7 +576,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -832,6 +840,1533 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I61"/>
   <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B6" sqref="B6"/>
+      <selection pane="topRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" style="7" customWidth="1"/>
+    <col min="2" max="5" width="10.44140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="7" customWidth="1"/>
+    <col min="7" max="8" width="10.33203125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="11.44140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="6" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+    </row>
+    <row r="4" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="41"/>
+      <c r="G4" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="20">
+        <v>6012</v>
+      </c>
+      <c r="C6" s="21">
+        <v>2937</v>
+      </c>
+      <c r="D6" s="22">
+        <v>3075</v>
+      </c>
+      <c r="E6" s="21">
+        <v>5497</v>
+      </c>
+      <c r="F6" s="22">
+        <v>515</v>
+      </c>
+      <c r="G6" s="21">
+        <v>22</v>
+      </c>
+      <c r="H6" s="21">
+        <v>714</v>
+      </c>
+      <c r="I6" s="21">
+        <v>5276</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="24">
+        <v>997</v>
+      </c>
+      <c r="C7" s="25">
+        <v>467</v>
+      </c>
+      <c r="D7" s="26">
+        <v>530</v>
+      </c>
+      <c r="E7" s="25">
+        <v>899</v>
+      </c>
+      <c r="F7" s="26">
+        <v>98</v>
+      </c>
+      <c r="G7" s="25">
+        <v>6</v>
+      </c>
+      <c r="H7" s="25">
+        <v>122</v>
+      </c>
+      <c r="I7" s="25">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="24">
+        <v>814</v>
+      </c>
+      <c r="C8" s="25">
+        <v>369</v>
+      </c>
+      <c r="D8" s="26">
+        <v>445</v>
+      </c>
+      <c r="E8" s="25">
+        <v>777</v>
+      </c>
+      <c r="F8" s="26">
+        <v>37</v>
+      </c>
+      <c r="G8" s="25">
+        <v>0</v>
+      </c>
+      <c r="H8" s="25">
+        <v>90</v>
+      </c>
+      <c r="I8" s="25">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="24">
+        <v>286</v>
+      </c>
+      <c r="C9" s="25">
+        <v>138</v>
+      </c>
+      <c r="D9" s="26">
+        <v>148</v>
+      </c>
+      <c r="E9" s="25">
+        <v>268</v>
+      </c>
+      <c r="F9" s="26">
+        <v>18</v>
+      </c>
+      <c r="G9" s="25">
+        <v>0</v>
+      </c>
+      <c r="H9" s="25">
+        <v>37</v>
+      </c>
+      <c r="I9" s="25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="24">
+        <v>25</v>
+      </c>
+      <c r="C10" s="25">
+        <v>16</v>
+      </c>
+      <c r="D10" s="26">
+        <v>9</v>
+      </c>
+      <c r="E10" s="25">
+        <v>25</v>
+      </c>
+      <c r="F10" s="26">
+        <v>0</v>
+      </c>
+      <c r="G10" s="25">
+        <v>0</v>
+      </c>
+      <c r="H10" s="25">
+        <v>1</v>
+      </c>
+      <c r="I10" s="25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="24">
+        <v>112</v>
+      </c>
+      <c r="C11" s="25">
+        <v>55</v>
+      </c>
+      <c r="D11" s="26">
+        <v>57</v>
+      </c>
+      <c r="E11" s="25">
+        <v>111</v>
+      </c>
+      <c r="F11" s="26">
+        <v>1</v>
+      </c>
+      <c r="G11" s="25">
+        <v>0</v>
+      </c>
+      <c r="H11" s="25">
+        <v>13</v>
+      </c>
+      <c r="I11" s="25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="24">
+        <v>37</v>
+      </c>
+      <c r="C12" s="25">
+        <v>18</v>
+      </c>
+      <c r="D12" s="26">
+        <v>19</v>
+      </c>
+      <c r="E12" s="25">
+        <v>35</v>
+      </c>
+      <c r="F12" s="26">
+        <v>2</v>
+      </c>
+      <c r="G12" s="25">
+        <v>0</v>
+      </c>
+      <c r="H12" s="25">
+        <v>7</v>
+      </c>
+      <c r="I12" s="25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="24">
+        <v>30</v>
+      </c>
+      <c r="C13" s="25">
+        <v>19</v>
+      </c>
+      <c r="D13" s="26">
+        <v>11</v>
+      </c>
+      <c r="E13" s="25">
+        <v>29</v>
+      </c>
+      <c r="F13" s="26">
+        <v>1</v>
+      </c>
+      <c r="G13" s="25">
+        <v>0</v>
+      </c>
+      <c r="H13" s="25">
+        <v>6</v>
+      </c>
+      <c r="I13" s="25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="24">
+        <v>34</v>
+      </c>
+      <c r="C14" s="25">
+        <v>20</v>
+      </c>
+      <c r="D14" s="26">
+        <v>14</v>
+      </c>
+      <c r="E14" s="25">
+        <v>33</v>
+      </c>
+      <c r="F14" s="26">
+        <v>1</v>
+      </c>
+      <c r="G14" s="25">
+        <v>0</v>
+      </c>
+      <c r="H14" s="25">
+        <v>3</v>
+      </c>
+      <c r="I14" s="25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="24">
+        <v>75</v>
+      </c>
+      <c r="C15" s="25">
+        <v>42</v>
+      </c>
+      <c r="D15" s="26">
+        <v>33</v>
+      </c>
+      <c r="E15" s="25">
+        <v>70</v>
+      </c>
+      <c r="F15" s="26">
+        <v>5</v>
+      </c>
+      <c r="G15" s="25">
+        <v>1</v>
+      </c>
+      <c r="H15" s="25">
+        <v>10</v>
+      </c>
+      <c r="I15" s="25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="24">
+        <v>196</v>
+      </c>
+      <c r="C16" s="25">
+        <v>110</v>
+      </c>
+      <c r="D16" s="26">
+        <v>86</v>
+      </c>
+      <c r="E16" s="25">
+        <v>192</v>
+      </c>
+      <c r="F16" s="26">
+        <v>4</v>
+      </c>
+      <c r="G16" s="25">
+        <v>0</v>
+      </c>
+      <c r="H16" s="25">
+        <v>26</v>
+      </c>
+      <c r="I16" s="25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="24">
+        <v>225</v>
+      </c>
+      <c r="C17" s="25">
+        <v>112</v>
+      </c>
+      <c r="D17" s="26">
+        <v>113</v>
+      </c>
+      <c r="E17" s="25">
+        <v>214</v>
+      </c>
+      <c r="F17" s="26">
+        <v>11</v>
+      </c>
+      <c r="G17" s="25">
+        <v>0</v>
+      </c>
+      <c r="H17" s="25">
+        <v>30</v>
+      </c>
+      <c r="I17" s="25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="24">
+        <v>186</v>
+      </c>
+      <c r="C18" s="25">
+        <v>85</v>
+      </c>
+      <c r="D18" s="26">
+        <v>101</v>
+      </c>
+      <c r="E18" s="25">
+        <v>174</v>
+      </c>
+      <c r="F18" s="26">
+        <v>12</v>
+      </c>
+      <c r="G18" s="25">
+        <v>1</v>
+      </c>
+      <c r="H18" s="25">
+        <v>15</v>
+      </c>
+      <c r="I18" s="25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="24">
+        <v>232</v>
+      </c>
+      <c r="C19" s="25">
+        <v>102</v>
+      </c>
+      <c r="D19" s="26">
+        <v>130</v>
+      </c>
+      <c r="E19" s="25">
+        <v>213</v>
+      </c>
+      <c r="F19" s="26">
+        <v>19</v>
+      </c>
+      <c r="G19" s="25">
+        <v>1</v>
+      </c>
+      <c r="H19" s="25">
+        <v>18</v>
+      </c>
+      <c r="I19" s="25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="24">
+        <v>67</v>
+      </c>
+      <c r="C20" s="25">
+        <v>33</v>
+      </c>
+      <c r="D20" s="26">
+        <v>34</v>
+      </c>
+      <c r="E20" s="25">
+        <v>58</v>
+      </c>
+      <c r="F20" s="26">
+        <v>9</v>
+      </c>
+      <c r="G20" s="25">
+        <v>0</v>
+      </c>
+      <c r="H20" s="25">
+        <v>14</v>
+      </c>
+      <c r="I20" s="25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="24">
+        <v>47</v>
+      </c>
+      <c r="C21" s="25">
+        <v>24</v>
+      </c>
+      <c r="D21" s="26">
+        <v>23</v>
+      </c>
+      <c r="E21" s="25">
+        <v>43</v>
+      </c>
+      <c r="F21" s="26">
+        <v>4</v>
+      </c>
+      <c r="G21" s="25">
+        <v>0</v>
+      </c>
+      <c r="H21" s="25">
+        <v>4</v>
+      </c>
+      <c r="I21" s="25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="24">
+        <v>11</v>
+      </c>
+      <c r="C22" s="25">
+        <v>4</v>
+      </c>
+      <c r="D22" s="26">
+        <v>7</v>
+      </c>
+      <c r="E22" s="25">
+        <v>10</v>
+      </c>
+      <c r="F22" s="26">
+        <v>1</v>
+      </c>
+      <c r="G22" s="25">
+        <v>0</v>
+      </c>
+      <c r="H22" s="25">
+        <v>0</v>
+      </c>
+      <c r="I22" s="25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="24">
+        <v>366</v>
+      </c>
+      <c r="C23" s="25">
+        <v>170</v>
+      </c>
+      <c r="D23" s="26">
+        <v>196</v>
+      </c>
+      <c r="E23" s="25">
+        <v>335</v>
+      </c>
+      <c r="F23" s="26">
+        <v>31</v>
+      </c>
+      <c r="G23" s="25">
+        <v>5</v>
+      </c>
+      <c r="H23" s="25">
+        <v>46</v>
+      </c>
+      <c r="I23" s="25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="24">
+        <v>149</v>
+      </c>
+      <c r="C24" s="25">
+        <v>77</v>
+      </c>
+      <c r="D24" s="26">
+        <v>72</v>
+      </c>
+      <c r="E24" s="25">
+        <v>136</v>
+      </c>
+      <c r="F24" s="26">
+        <v>13</v>
+      </c>
+      <c r="G24" s="25">
+        <v>0</v>
+      </c>
+      <c r="H24" s="25">
+        <v>23</v>
+      </c>
+      <c r="I24" s="25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="24">
+        <v>442</v>
+      </c>
+      <c r="C25" s="25">
+        <v>241</v>
+      </c>
+      <c r="D25" s="26">
+        <v>201</v>
+      </c>
+      <c r="E25" s="25">
+        <v>405</v>
+      </c>
+      <c r="F25" s="26">
+        <v>37</v>
+      </c>
+      <c r="G25" s="25">
+        <v>3</v>
+      </c>
+      <c r="H25" s="25">
+        <v>52</v>
+      </c>
+      <c r="I25" s="25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="24">
+        <v>160</v>
+      </c>
+      <c r="C26" s="25">
+        <v>91</v>
+      </c>
+      <c r="D26" s="26">
+        <v>69</v>
+      </c>
+      <c r="E26" s="25">
+        <v>143</v>
+      </c>
+      <c r="F26" s="26">
+        <v>17</v>
+      </c>
+      <c r="G26" s="25">
+        <v>0</v>
+      </c>
+      <c r="H26" s="25">
+        <v>17</v>
+      </c>
+      <c r="I26" s="25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="24">
+        <v>272</v>
+      </c>
+      <c r="C27" s="25">
+        <v>136</v>
+      </c>
+      <c r="D27" s="26">
+        <v>136</v>
+      </c>
+      <c r="E27" s="25">
+        <v>234</v>
+      </c>
+      <c r="F27" s="26">
+        <v>38</v>
+      </c>
+      <c r="G27" s="25">
+        <v>1</v>
+      </c>
+      <c r="H27" s="25">
+        <v>25</v>
+      </c>
+      <c r="I27" s="25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="24">
+        <v>469</v>
+      </c>
+      <c r="C28" s="25">
+        <v>225</v>
+      </c>
+      <c r="D28" s="26">
+        <v>244</v>
+      </c>
+      <c r="E28" s="25">
+        <v>417</v>
+      </c>
+      <c r="F28" s="26">
+        <v>52</v>
+      </c>
+      <c r="G28" s="25">
+        <v>0</v>
+      </c>
+      <c r="H28" s="25">
+        <v>59</v>
+      </c>
+      <c r="I28" s="25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="24">
+        <v>250</v>
+      </c>
+      <c r="C29" s="25">
+        <v>135</v>
+      </c>
+      <c r="D29" s="26">
+        <v>115</v>
+      </c>
+      <c r="E29" s="25">
+        <v>229</v>
+      </c>
+      <c r="F29" s="26">
+        <v>21</v>
+      </c>
+      <c r="G29" s="25">
+        <v>1</v>
+      </c>
+      <c r="H29" s="25">
+        <v>36</v>
+      </c>
+      <c r="I29" s="25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="24">
+        <v>144</v>
+      </c>
+      <c r="C30" s="25">
+        <v>70</v>
+      </c>
+      <c r="D30" s="26">
+        <v>74</v>
+      </c>
+      <c r="E30" s="25">
+        <v>133</v>
+      </c>
+      <c r="F30" s="26">
+        <v>11</v>
+      </c>
+      <c r="G30" s="25">
+        <v>2</v>
+      </c>
+      <c r="H30" s="25">
+        <v>15</v>
+      </c>
+      <c r="I30" s="25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="24">
+        <v>325</v>
+      </c>
+      <c r="C31" s="25">
+        <v>151</v>
+      </c>
+      <c r="D31" s="26">
+        <v>174</v>
+      </c>
+      <c r="E31" s="25">
+        <v>256</v>
+      </c>
+      <c r="F31" s="26">
+        <v>69</v>
+      </c>
+      <c r="G31" s="25">
+        <v>1</v>
+      </c>
+      <c r="H31" s="25">
+        <v>35</v>
+      </c>
+      <c r="I31" s="25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="24">
+        <v>61</v>
+      </c>
+      <c r="C32" s="25">
+        <v>27</v>
+      </c>
+      <c r="D32" s="27">
+        <v>34</v>
+      </c>
+      <c r="E32" s="25">
+        <v>58</v>
+      </c>
+      <c r="F32" s="27">
+        <v>3</v>
+      </c>
+      <c r="G32" s="25">
+        <v>0</v>
+      </c>
+      <c r="H32" s="25">
+        <v>10</v>
+      </c>
+      <c r="I32" s="25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+    </row>
+    <row r="34" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="25">
+        <v>302</v>
+      </c>
+      <c r="C34" s="25">
+        <v>135</v>
+      </c>
+      <c r="D34" s="31">
+        <v>167</v>
+      </c>
+      <c r="E34" s="25">
+        <v>274</v>
+      </c>
+      <c r="F34" s="31">
+        <v>28</v>
+      </c>
+      <c r="G34" s="25">
+        <v>5</v>
+      </c>
+      <c r="H34" s="25">
+        <v>36</v>
+      </c>
+      <c r="I34" s="25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="25">
+        <v>140</v>
+      </c>
+      <c r="C35" s="25">
+        <v>69</v>
+      </c>
+      <c r="D35" s="26">
+        <v>71</v>
+      </c>
+      <c r="E35" s="25">
+        <v>109</v>
+      </c>
+      <c r="F35" s="26">
+        <v>31</v>
+      </c>
+      <c r="G35" s="25">
+        <v>0</v>
+      </c>
+      <c r="H35" s="25">
+        <v>21</v>
+      </c>
+      <c r="I35" s="25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="25">
+        <v>161</v>
+      </c>
+      <c r="C36" s="25">
+        <v>74</v>
+      </c>
+      <c r="D36" s="26">
+        <v>87</v>
+      </c>
+      <c r="E36" s="25">
+        <v>149</v>
+      </c>
+      <c r="F36" s="26">
+        <v>12</v>
+      </c>
+      <c r="G36" s="25">
+        <v>1</v>
+      </c>
+      <c r="H36" s="25">
+        <v>13</v>
+      </c>
+      <c r="I36" s="25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="25">
+        <v>99</v>
+      </c>
+      <c r="C37" s="25">
+        <v>36</v>
+      </c>
+      <c r="D37" s="26">
+        <v>63</v>
+      </c>
+      <c r="E37" s="25">
+        <v>91</v>
+      </c>
+      <c r="F37" s="26">
+        <v>8</v>
+      </c>
+      <c r="G37" s="25">
+        <v>0</v>
+      </c>
+      <c r="H37" s="25">
+        <v>8</v>
+      </c>
+      <c r="I37" s="25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="25">
+        <v>92</v>
+      </c>
+      <c r="C38" s="25">
+        <v>47</v>
+      </c>
+      <c r="D38" s="26">
+        <v>45</v>
+      </c>
+      <c r="E38" s="25">
+        <v>79</v>
+      </c>
+      <c r="F38" s="26">
+        <v>13</v>
+      </c>
+      <c r="G38" s="25">
+        <v>0</v>
+      </c>
+      <c r="H38" s="25">
+        <v>12</v>
+      </c>
+      <c r="I38" s="25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="25">
+        <v>75</v>
+      </c>
+      <c r="C39" s="25">
+        <v>35</v>
+      </c>
+      <c r="D39" s="26">
+        <v>40</v>
+      </c>
+      <c r="E39" s="25">
+        <v>69</v>
+      </c>
+      <c r="F39" s="26">
+        <v>6</v>
+      </c>
+      <c r="G39" s="25">
+        <v>0</v>
+      </c>
+      <c r="H39" s="25">
+        <v>13</v>
+      </c>
+      <c r="I39" s="25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="25">
+        <v>50</v>
+      </c>
+      <c r="C40" s="25">
+        <v>20</v>
+      </c>
+      <c r="D40" s="26">
+        <v>30</v>
+      </c>
+      <c r="E40" s="25">
+        <v>47</v>
+      </c>
+      <c r="F40" s="26">
+        <v>3</v>
+      </c>
+      <c r="G40" s="25">
+        <v>0</v>
+      </c>
+      <c r="H40" s="25">
+        <v>8</v>
+      </c>
+      <c r="I40" s="25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="25">
+        <v>71</v>
+      </c>
+      <c r="C41" s="25">
+        <v>28</v>
+      </c>
+      <c r="D41" s="26">
+        <v>43</v>
+      </c>
+      <c r="E41" s="25">
+        <v>69</v>
+      </c>
+      <c r="F41" s="26">
+        <v>2</v>
+      </c>
+      <c r="G41" s="25">
+        <v>0</v>
+      </c>
+      <c r="H41" s="25">
+        <v>2</v>
+      </c>
+      <c r="I41" s="25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="25">
+        <v>49</v>
+      </c>
+      <c r="C42" s="25">
+        <v>26</v>
+      </c>
+      <c r="D42" s="26">
+        <v>23</v>
+      </c>
+      <c r="E42" s="25">
+        <v>41</v>
+      </c>
+      <c r="F42" s="26">
+        <v>8</v>
+      </c>
+      <c r="G42" s="25">
+        <v>0</v>
+      </c>
+      <c r="H42" s="25">
+        <v>3</v>
+      </c>
+      <c r="I42" s="25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="25">
+        <v>53</v>
+      </c>
+      <c r="C43" s="25">
+        <v>20</v>
+      </c>
+      <c r="D43" s="26">
+        <v>33</v>
+      </c>
+      <c r="E43" s="25">
+        <v>49</v>
+      </c>
+      <c r="F43" s="26">
+        <v>4</v>
+      </c>
+      <c r="G43" s="25">
+        <v>0</v>
+      </c>
+      <c r="H43" s="25">
+        <v>5</v>
+      </c>
+      <c r="I43" s="25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="25">
+        <v>36</v>
+      </c>
+      <c r="C44" s="25">
+        <v>12</v>
+      </c>
+      <c r="D44" s="26">
+        <v>24</v>
+      </c>
+      <c r="E44" s="25">
+        <v>33</v>
+      </c>
+      <c r="F44" s="26">
+        <v>3</v>
+      </c>
+      <c r="G44" s="25">
+        <v>0</v>
+      </c>
+      <c r="H44" s="25">
+        <v>3</v>
+      </c>
+      <c r="I44" s="25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="25">
+        <v>33</v>
+      </c>
+      <c r="C45" s="25">
+        <v>14</v>
+      </c>
+      <c r="D45" s="26">
+        <v>19</v>
+      </c>
+      <c r="E45" s="25">
+        <v>31</v>
+      </c>
+      <c r="F45" s="26">
+        <v>2</v>
+      </c>
+      <c r="G45" s="25">
+        <v>0</v>
+      </c>
+      <c r="H45" s="25">
+        <v>3</v>
+      </c>
+      <c r="I45" s="25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="25">
+        <v>36</v>
+      </c>
+      <c r="C46" s="25">
+        <v>22</v>
+      </c>
+      <c r="D46" s="26">
+        <v>14</v>
+      </c>
+      <c r="E46" s="25">
+        <v>32</v>
+      </c>
+      <c r="F46" s="26">
+        <v>4</v>
+      </c>
+      <c r="G46" s="25">
+        <v>0</v>
+      </c>
+      <c r="H46" s="25">
+        <v>5</v>
+      </c>
+      <c r="I46" s="25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="25">
+        <v>33</v>
+      </c>
+      <c r="C47" s="25">
+        <v>13</v>
+      </c>
+      <c r="D47" s="26">
+        <v>20</v>
+      </c>
+      <c r="E47" s="25">
+        <v>27</v>
+      </c>
+      <c r="F47" s="26">
+        <v>6</v>
+      </c>
+      <c r="G47" s="25">
+        <v>0</v>
+      </c>
+      <c r="H47" s="25">
+        <v>6</v>
+      </c>
+      <c r="I47" s="25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="25">
+        <v>28</v>
+      </c>
+      <c r="C48" s="25">
+        <v>15</v>
+      </c>
+      <c r="D48" s="26">
+        <v>13</v>
+      </c>
+      <c r="E48" s="25">
+        <v>27</v>
+      </c>
+      <c r="F48" s="26">
+        <v>1</v>
+      </c>
+      <c r="G48" s="25">
+        <v>0</v>
+      </c>
+      <c r="H48" s="25">
+        <v>5</v>
+      </c>
+      <c r="I48" s="25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="25">
+        <v>41</v>
+      </c>
+      <c r="C49" s="25">
+        <v>18</v>
+      </c>
+      <c r="D49" s="26">
+        <v>23</v>
+      </c>
+      <c r="E49" s="25">
+        <v>38</v>
+      </c>
+      <c r="F49" s="26">
+        <v>3</v>
+      </c>
+      <c r="G49" s="25">
+        <v>0</v>
+      </c>
+      <c r="H49" s="25">
+        <v>5</v>
+      </c>
+      <c r="I49" s="25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" s="25">
+        <v>33</v>
+      </c>
+      <c r="C50" s="25">
+        <v>16</v>
+      </c>
+      <c r="D50" s="26">
+        <v>17</v>
+      </c>
+      <c r="E50" s="25">
+        <v>30</v>
+      </c>
+      <c r="F50" s="26">
+        <v>3</v>
+      </c>
+      <c r="G50" s="25">
+        <v>0</v>
+      </c>
+      <c r="H50" s="25">
+        <v>2</v>
+      </c>
+      <c r="I50" s="25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="25">
+        <v>13</v>
+      </c>
+      <c r="C51" s="25">
+        <v>4</v>
+      </c>
+      <c r="D51" s="26">
+        <v>9</v>
+      </c>
+      <c r="E51" s="25">
+        <v>9</v>
+      </c>
+      <c r="F51" s="26">
+        <v>4</v>
+      </c>
+      <c r="G51" s="25">
+        <v>0</v>
+      </c>
+      <c r="H51" s="25">
+        <v>2</v>
+      </c>
+      <c r="I51" s="25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="24">
+        <v>23</v>
+      </c>
+      <c r="C52" s="25">
+        <v>8</v>
+      </c>
+      <c r="D52" s="26">
+        <v>15</v>
+      </c>
+      <c r="E52" s="25">
+        <v>19</v>
+      </c>
+      <c r="F52" s="26">
+        <v>4</v>
+      </c>
+      <c r="G52" s="25">
+        <v>1</v>
+      </c>
+      <c r="H52" s="25">
+        <v>5</v>
+      </c>
+      <c r="I52" s="25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="32">
+        <v>30</v>
+      </c>
+      <c r="C53" s="33">
+        <v>17</v>
+      </c>
+      <c r="D53" s="27">
+        <v>13</v>
+      </c>
+      <c r="E53" s="33">
+        <v>25</v>
+      </c>
+      <c r="F53" s="27">
+        <v>5</v>
+      </c>
+      <c r="G53" s="33">
+        <v>0</v>
+      </c>
+      <c r="H53" s="33">
+        <v>4</v>
+      </c>
+      <c r="I53" s="33">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" s="35"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" s="37"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C56" s="37"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="36"/>
+      <c r="C57" s="37"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I61"/>
+  <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B6" sqref="B6"/>
@@ -855,7 +2390,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -941,28 +2476,28 @@
         <v>9</v>
       </c>
       <c r="B6" s="20">
-        <v>6012</v>
+        <v>5556</v>
       </c>
       <c r="C6" s="21">
-        <v>2937</v>
+        <v>2652</v>
       </c>
       <c r="D6" s="22">
-        <v>3075</v>
+        <v>2904</v>
       </c>
       <c r="E6" s="21">
-        <v>5497</v>
+        <v>5097</v>
       </c>
       <c r="F6" s="22">
-        <v>515</v>
+        <v>459</v>
       </c>
       <c r="G6" s="21">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H6" s="21">
-        <v>714</v>
+        <v>685</v>
       </c>
       <c r="I6" s="21">
-        <v>5276</v>
+        <v>4848</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -970,28 +2505,28 @@
         <v>11</v>
       </c>
       <c r="B7" s="24">
-        <v>997</v>
+        <v>860</v>
       </c>
       <c r="C7" s="25">
-        <v>467</v>
+        <v>412</v>
       </c>
       <c r="D7" s="26">
-        <v>530</v>
+        <v>448</v>
       </c>
       <c r="E7" s="25">
-        <v>899</v>
+        <v>780</v>
       </c>
       <c r="F7" s="26">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="G7" s="25">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H7" s="25">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="I7" s="25">
-        <v>869</v>
+        <v>760</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -999,28 +2534,28 @@
         <v>12</v>
       </c>
       <c r="B8" s="24">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="C8" s="25">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D8" s="26">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="E8" s="25">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="F8" s="26">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G8" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="25">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="I8" s="25">
-        <v>724</v>
+        <v>685</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1028,28 +2563,28 @@
         <v>13</v>
       </c>
       <c r="B9" s="24">
-        <v>286</v>
+        <v>248</v>
       </c>
       <c r="C9" s="25">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="D9" s="26">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E9" s="25">
-        <v>268</v>
+        <v>237</v>
       </c>
       <c r="F9" s="26">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G9" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="25">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="I9" s="25">
-        <v>249</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1060,25 +2595,25 @@
         <v>25</v>
       </c>
       <c r="C10" s="25">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" s="26">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E10" s="25">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F10" s="26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G10" s="25">
         <v>0</v>
       </c>
       <c r="H10" s="25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I10" s="25">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1086,28 +2621,28 @@
         <v>15</v>
       </c>
       <c r="B11" s="24">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="C11" s="25">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D11" s="26">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="E11" s="25">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="F11" s="26">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G11" s="25">
         <v>0</v>
       </c>
       <c r="H11" s="25">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I11" s="25">
-        <v>99</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1115,28 +2650,28 @@
         <v>16</v>
       </c>
       <c r="B12" s="24">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C12" s="25">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D12" s="26">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E12" s="25">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F12" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="25">
         <v>0</v>
       </c>
       <c r="H12" s="25">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I12" s="25">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1144,28 +2679,28 @@
         <v>17</v>
       </c>
       <c r="B13" s="24">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C13" s="25">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D13" s="26">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E13" s="25">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F13" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="25">
         <v>0</v>
       </c>
       <c r="H13" s="25">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I13" s="25">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1173,28 +2708,28 @@
         <v>18</v>
       </c>
       <c r="B14" s="24">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C14" s="25">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D14" s="26">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E14" s="25">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F14" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="25">
         <v>0</v>
       </c>
       <c r="H14" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I14" s="25">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1202,28 +2737,28 @@
         <v>19</v>
       </c>
       <c r="B15" s="24">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C15" s="25">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D15" s="26">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="25">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="F15" s="26">
         <v>5</v>
       </c>
       <c r="G15" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="25">
         <v>10</v>
       </c>
       <c r="I15" s="25">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1231,28 +2766,28 @@
         <v>20</v>
       </c>
       <c r="B16" s="24">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="C16" s="25">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="D16" s="26">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E16" s="25">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="F16" s="26">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G16" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="25">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I16" s="25">
-        <v>170</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1260,28 +2795,28 @@
         <v>21</v>
       </c>
       <c r="B17" s="24">
-        <v>225</v>
+        <v>181</v>
       </c>
       <c r="C17" s="25">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="D17" s="26">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E17" s="25">
-        <v>214</v>
+        <v>174</v>
       </c>
       <c r="F17" s="26">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G17" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="25">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="I17" s="25">
-        <v>195</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1289,28 +2824,28 @@
         <v>22</v>
       </c>
       <c r="B18" s="24">
-        <v>186</v>
+        <v>147</v>
       </c>
       <c r="C18" s="25">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D18" s="26">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="E18" s="25">
-        <v>174</v>
+        <v>138</v>
       </c>
       <c r="F18" s="26">
+        <v>9</v>
+      </c>
+      <c r="G18" s="25">
+        <v>0</v>
+      </c>
+      <c r="H18" s="25">
         <v>12</v>
       </c>
-      <c r="G18" s="25">
-        <v>1</v>
-      </c>
-      <c r="H18" s="25">
-        <v>15</v>
-      </c>
       <c r="I18" s="25">
-        <v>170</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1318,28 +2853,28 @@
         <v>23</v>
       </c>
       <c r="B19" s="24">
-        <v>232</v>
+        <v>203</v>
       </c>
       <c r="C19" s="25">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D19" s="26">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="E19" s="25">
-        <v>213</v>
+        <v>188</v>
       </c>
       <c r="F19" s="26">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G19" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="25">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I19" s="25">
-        <v>213</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1347,28 +2882,28 @@
         <v>24</v>
       </c>
       <c r="B20" s="24">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C20" s="25">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="26">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E20" s="25">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F20" s="26">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G20" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="25">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="I20" s="25">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1376,28 +2911,28 @@
         <v>25</v>
       </c>
       <c r="B21" s="24">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" s="25">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D21" s="26">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E21" s="25">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F21" s="26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G21" s="25">
         <v>0</v>
       </c>
       <c r="H21" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I21" s="25">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1405,25 +2940,25 @@
         <v>26</v>
       </c>
       <c r="B22" s="24">
+        <v>13</v>
+      </c>
+      <c r="C22" s="25">
+        <v>5</v>
+      </c>
+      <c r="D22" s="26">
+        <v>8</v>
+      </c>
+      <c r="E22" s="25">
         <v>11</v>
       </c>
-      <c r="C22" s="25">
-        <v>4</v>
-      </c>
-      <c r="D22" s="26">
-        <v>7</v>
-      </c>
-      <c r="E22" s="25">
-        <v>10</v>
-      </c>
       <c r="F22" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G22" s="25">
         <v>0</v>
       </c>
       <c r="H22" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I22" s="25">
         <v>11</v>
@@ -1434,28 +2969,28 @@
         <v>27</v>
       </c>
       <c r="B23" s="24">
-        <v>366</v>
+        <v>340</v>
       </c>
       <c r="C23" s="25">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="D23" s="26">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="E23" s="25">
-        <v>335</v>
+        <v>301</v>
       </c>
       <c r="F23" s="26">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G23" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H23" s="25">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I23" s="25">
-        <v>315</v>
+        <v>289</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1463,28 +2998,28 @@
         <v>28</v>
       </c>
       <c r="B24" s="24">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C24" s="25">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D24" s="26">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="E24" s="25">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="F24" s="26">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G24" s="25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H24" s="25">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I24" s="25">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1492,28 +3027,28 @@
         <v>29</v>
       </c>
       <c r="B25" s="24">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="C25" s="25">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="D25" s="26">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="E25" s="25">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="F25" s="26">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G25" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H25" s="25">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I25" s="25">
-        <v>387</v>
+        <v>395</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1521,25 +3056,25 @@
         <v>30</v>
       </c>
       <c r="B26" s="24">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C26" s="25">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D26" s="26">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="E26" s="25">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="F26" s="26">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G26" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H26" s="25">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="I26" s="25">
         <v>143</v>
@@ -1550,28 +3085,28 @@
         <v>31</v>
       </c>
       <c r="B27" s="24">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C27" s="25">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="D27" s="26">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="E27" s="25">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="F27" s="26">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G27" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" s="25">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I27" s="25">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1579,28 +3114,28 @@
         <v>32</v>
       </c>
       <c r="B28" s="24">
-        <v>469</v>
+        <v>448</v>
       </c>
       <c r="C28" s="25">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="D28" s="26">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E28" s="25">
-        <v>417</v>
+        <v>391</v>
       </c>
       <c r="F28" s="26">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G28" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H28" s="25">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I28" s="25">
-        <v>410</v>
+        <v>388</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1608,28 +3143,28 @@
         <v>33</v>
       </c>
       <c r="B29" s="24">
-        <v>250</v>
+        <v>229</v>
       </c>
       <c r="C29" s="25">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="D29" s="26">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E29" s="25">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="F29" s="26">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G29" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="25">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I29" s="25">
-        <v>213</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1637,28 +3172,28 @@
         <v>34</v>
       </c>
       <c r="B30" s="24">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C30" s="25">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D30" s="26">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E30" s="25">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="F30" s="26">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G30" s="25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H30" s="25">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I30" s="25">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1666,28 +3201,28 @@
         <v>35</v>
       </c>
       <c r="B31" s="24">
-        <v>325</v>
+        <v>293</v>
       </c>
       <c r="C31" s="25">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D31" s="26">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="E31" s="25">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="F31" s="26">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="G31" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H31" s="25">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I31" s="25">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1695,28 +3230,28 @@
         <v>36</v>
       </c>
       <c r="B32" s="24">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C32" s="25">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D32" s="27">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E32" s="25">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="F32" s="27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G32" s="25">
         <v>0</v>
       </c>
       <c r="H32" s="25">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I32" s="25">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1737,28 +3272,28 @@
         <v>11</v>
       </c>
       <c r="B34" s="25">
-        <v>302</v>
+        <v>243</v>
       </c>
       <c r="C34" s="25">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="D34" s="31">
-        <v>167</v>
+        <v>136</v>
       </c>
       <c r="E34" s="25">
-        <v>274</v>
+        <v>218</v>
       </c>
       <c r="F34" s="31">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G34" s="25">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H34" s="25">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="I34" s="25">
-        <v>261</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1766,28 +3301,28 @@
         <v>35</v>
       </c>
       <c r="B35" s="25">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="C35" s="25">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D35" s="26">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E35" s="25">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F35" s="26">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G35" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="25">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I35" s="25">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1795,28 +3330,28 @@
         <v>38</v>
       </c>
       <c r="B36" s="25">
-        <v>161</v>
+        <v>124</v>
       </c>
       <c r="C36" s="25">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D36" s="26">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="E36" s="25">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="F36" s="26">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G36" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" s="25">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I36" s="25">
-        <v>147</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1824,28 +3359,28 @@
         <v>12</v>
       </c>
       <c r="B37" s="25">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C37" s="25">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D37" s="26">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E37" s="25">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F37" s="26">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G37" s="25">
         <v>0</v>
       </c>
       <c r="H37" s="25">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I37" s="25">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1853,28 +3388,28 @@
         <v>39</v>
       </c>
       <c r="B38" s="25">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="C38" s="25">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D38" s="26">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E38" s="25">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="F38" s="26">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G38" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="25">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I38" s="25">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1885,10 +3420,10 @@
         <v>75</v>
       </c>
       <c r="C39" s="25">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D39" s="26">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E39" s="25">
         <v>69</v>
@@ -1897,13 +3432,13 @@
         <v>6</v>
       </c>
       <c r="G39" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="25">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I39" s="25">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1911,28 +3446,28 @@
         <v>27</v>
       </c>
       <c r="B40" s="25">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C40" s="25">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D40" s="26">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E40" s="25">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F40" s="26">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G40" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="25">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I40" s="25">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1940,28 +3475,28 @@
         <v>13</v>
       </c>
       <c r="B41" s="25">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C41" s="25">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D41" s="26">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E41" s="25">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="F41" s="26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G41" s="25">
         <v>0</v>
       </c>
       <c r="H41" s="25">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I41" s="25">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1969,28 +3504,28 @@
         <v>41</v>
       </c>
       <c r="B42" s="25">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C42" s="25">
+        <v>18</v>
+      </c>
+      <c r="D42" s="26">
         <v>26</v>
       </c>
-      <c r="D42" s="26">
-        <v>23</v>
-      </c>
       <c r="E42" s="25">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F42" s="26">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G42" s="25">
         <v>0</v>
       </c>
       <c r="H42" s="25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I42" s="25">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1998,28 +3533,28 @@
         <v>42</v>
       </c>
       <c r="B43" s="25">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C43" s="25">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D43" s="26">
         <v>33</v>
       </c>
       <c r="E43" s="25">
+        <v>57</v>
+      </c>
+      <c r="F43" s="26">
+        <v>3</v>
+      </c>
+      <c r="G43" s="25">
+        <v>0</v>
+      </c>
+      <c r="H43" s="25">
+        <v>11</v>
+      </c>
+      <c r="I43" s="25">
         <v>49</v>
-      </c>
-      <c r="F43" s="26">
-        <v>4</v>
-      </c>
-      <c r="G43" s="25">
-        <v>0</v>
-      </c>
-      <c r="H43" s="25">
-        <v>5</v>
-      </c>
-      <c r="I43" s="25">
-        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2027,28 +3562,28 @@
         <v>43</v>
       </c>
       <c r="B44" s="25">
+        <v>44</v>
+      </c>
+      <c r="C44" s="25">
+        <v>22</v>
+      </c>
+      <c r="D44" s="26">
+        <v>22</v>
+      </c>
+      <c r="E44" s="25">
+        <v>43</v>
+      </c>
+      <c r="F44" s="26">
+        <v>1</v>
+      </c>
+      <c r="G44" s="25">
+        <v>0</v>
+      </c>
+      <c r="H44" s="25">
+        <v>8</v>
+      </c>
+      <c r="I44" s="25">
         <v>36</v>
-      </c>
-      <c r="C44" s="25">
-        <v>12</v>
-      </c>
-      <c r="D44" s="26">
-        <v>24</v>
-      </c>
-      <c r="E44" s="25">
-        <v>33</v>
-      </c>
-      <c r="F44" s="26">
-        <v>3</v>
-      </c>
-      <c r="G44" s="25">
-        <v>0</v>
-      </c>
-      <c r="H44" s="25">
-        <v>3</v>
-      </c>
-      <c r="I44" s="25">
-        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2056,28 +3591,28 @@
         <v>44</v>
       </c>
       <c r="B45" s="25">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C45" s="25">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D45" s="26">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E45" s="25">
+        <v>34</v>
+      </c>
+      <c r="F45" s="26">
+        <v>1</v>
+      </c>
+      <c r="G45" s="25">
+        <v>0</v>
+      </c>
+      <c r="H45" s="25">
+        <v>4</v>
+      </c>
+      <c r="I45" s="25">
         <v>31</v>
-      </c>
-      <c r="F45" s="26">
-        <v>2</v>
-      </c>
-      <c r="G45" s="25">
-        <v>0</v>
-      </c>
-      <c r="H45" s="25">
-        <v>3</v>
-      </c>
-      <c r="I45" s="25">
-        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2085,28 +3620,28 @@
         <v>45</v>
       </c>
       <c r="B46" s="25">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C46" s="25">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D46" s="26">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E46" s="25">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F46" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G46" s="25">
         <v>0</v>
       </c>
       <c r="H46" s="25">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I46" s="25">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2114,28 +3649,28 @@
         <v>24</v>
       </c>
       <c r="B47" s="25">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C47" s="25">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D47" s="26">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E47" s="25">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F47" s="26">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G47" s="25">
         <v>0</v>
       </c>
       <c r="H47" s="25">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I47" s="25">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2143,28 +3678,28 @@
         <v>46</v>
       </c>
       <c r="B48" s="25">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C48" s="25">
+        <v>11</v>
+      </c>
+      <c r="D48" s="26">
         <v>15</v>
       </c>
-      <c r="D48" s="26">
-        <v>13</v>
-      </c>
       <c r="E48" s="25">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F48" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G48" s="25">
         <v>0</v>
       </c>
       <c r="H48" s="25">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I48" s="25">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="21.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2172,28 +3707,28 @@
         <v>47</v>
       </c>
       <c r="B49" s="25">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C49" s="25">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D49" s="26">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E49" s="25">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F49" s="26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G49" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H49" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I49" s="25">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2201,28 +3736,28 @@
         <v>34</v>
       </c>
       <c r="B50" s="25">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C50" s="25">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D50" s="26">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E50" s="25">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F50" s="26">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G50" s="25">
         <v>0</v>
       </c>
       <c r="H50" s="25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I50" s="25">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2230,28 +3765,28 @@
         <v>48</v>
       </c>
       <c r="B51" s="25">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C51" s="25">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D51" s="26">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E51" s="25">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F51" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G51" s="25">
         <v>0</v>
       </c>
       <c r="H51" s="25">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I51" s="25">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2259,25 +3794,25 @@
         <v>49</v>
       </c>
       <c r="B52" s="24">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C52" s="25">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D52" s="26">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E52" s="25">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F52" s="26">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G52" s="25">
+        <v>0</v>
+      </c>
+      <c r="H52" s="25">
         <v>1</v>
-      </c>
-      <c r="H52" s="25">
-        <v>5</v>
       </c>
       <c r="I52" s="25">
         <v>17</v>
@@ -2288,33 +3823,33 @@
         <v>50</v>
       </c>
       <c r="B53" s="32">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C53" s="33">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D53" s="27">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E53" s="33">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F53" s="27">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G53" s="33">
         <v>0</v>
       </c>
       <c r="H53" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I53" s="33">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="34" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B54" s="35"/>
       <c r="C54" s="35"/>

</xml_diff>